<commit_message>
Update Gestion De Ressources
Modification Gestion de Ressources pour Macro
</commit_message>
<xml_diff>
--- a/ressources/Gestion-De-Ressources.xlsx
+++ b/ressources/Gestion-De-Ressources.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Wamp64\www\sites\P2\DISII-Projet2\ressources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\sites\p2\DISII-Projet2\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="home" sheetId="1" r:id="rId1"/>
     <sheet name="documents" sheetId="3" r:id="rId2"/>
-    <sheet name="Feuil1" sheetId="4" r:id="rId3"/>
-    <sheet name="settings" sheetId="2" r:id="rId4"/>
+    <sheet name="settings" sheetId="2" r:id="rId3"/>
+    <sheet name="listing" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="auteur">settings!$H$2:OFFSET(settings!$H$2,settings!$I$1-1,,)</definedName>
     <definedName name="categories">settings!$J$2:OFFSET(settings!$J$2,settings!$K$1-1,,)</definedName>
+    <definedName name="listingvba">listing!$A$2:OFFSET(listing!$A$2,listing!$G$2-1,,)</definedName>
     <definedName name="statut">settings!$F$2:OFFSET(settings!$F$2,settings!$G$1-1,,)</definedName>
     <definedName name="themes">settings!$L$2:OFFSET(settings!$L$2,settings!$M$1-1,,)</definedName>
     <definedName name="type">settings!$D$2:OFFSET(settings!$D$2,settings!$E$1-1,,)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
   <si>
     <t>MENU</t>
   </si>
@@ -225,26 +226,47 @@
     <t>text/php</t>
   </si>
   <si>
-    <t>hjgfhfg</t>
-  </si>
-  <si>
-    <t>dqsd</t>
-  </si>
-  <si>
-    <t>qsd</t>
-  </si>
-  <si>
-    <t>http://forum.telecharger.01net.com/forum/high-tech/LOGICIELS/Developpement/resolu-fichiers-excel-sujet_175112_1.htm</t>
+    <t>C:\wamp64\www\sites\p2\DISII-Projet2\ressources\</t>
+  </si>
+  <si>
+    <t>Sujet Projet 02.pdf</t>
+  </si>
+  <si>
+    <t>Projet – Site Statique.pptx</t>
+  </si>
+  <si>
+    <t>Suivi_aSlimani_V2.xlsx</t>
+  </si>
+  <si>
+    <t>Charte Graphique Mockup et Annexe.pdf</t>
+  </si>
+  <si>
+    <t>Charte Graphique.docx</t>
+  </si>
+  <si>
+    <t>Charte Graphique.pdf</t>
+  </si>
+  <si>
+    <t>Mockup_Makit.pdf</t>
+  </si>
+  <si>
+    <t>Caché</t>
+  </si>
+  <si>
+    <t>date d'accès</t>
+  </si>
+  <si>
+    <t>~$Suivi_aSlimani_V2.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; octets&quot;"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,20 +317,69 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -318,7 +389,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -329,20 +400,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -350,18 +434,158 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Texte explicatif" xfId="1" builtinId="53"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="16">
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
-        <color theme="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="0&quot; octets&quot;"/>
       <fill>
-        <patternFill>
-          <bgColor theme="8"/>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -389,55 +613,395 @@
         <sz val="11"/>
         <color theme="0"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="164" formatCode="0&quot; octets&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0&quot; octets&quot;"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -452,29 +1016,116 @@
 </styleSheet>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>19050</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>752475</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Button 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03619B50-4563-4801-8682-C10CF0EF7454}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="fr-FR" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri"/>
+                  <a:cs typeface="Calibri"/>
+                </a:rPr>
+                <a:t>Actualiser</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="listingdocuments" displayName="listingdocuments" ref="A1:M5" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:M5"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:N4" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A1:N4"/>
+  <tableColumns count="14">
     <tableColumn id="1" name="id" dataDxfId="14">
       <calculatedColumnFormula>IF(NOT(ISBLANK(B2)),CONCATENATE(settings!$A$2,settings!B2),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="nom de fichier" dataDxfId="13"/>
     <tableColumn id="3" name="description" dataDxfId="12"/>
     <tableColumn id="4" name="type" dataDxfId="11"/>
-    <tableColumn id="5" name="date de création" dataDxfId="10"/>
-    <tableColumn id="6" name="date de modification" dataDxfId="9"/>
-    <tableColumn id="7" name="auteur" dataDxfId="8"/>
-    <tableColumn id="8" name="catégories" dataDxfId="7"/>
-    <tableColumn id="9" name="thèmes" dataDxfId="6"/>
-    <tableColumn id="10" name="statut" dataDxfId="5"/>
-    <tableColumn id="11" name="taille" dataDxfId="4"/>
-    <tableColumn id="12" name="emplacement" dataDxfId="3"/>
-    <tableColumn id="13" name="afficher" dataDxfId="2" dataCellStyle="Lien hypertexte">
-      <calculatedColumnFormula>IF(AND(B2&lt;&gt;"",L2&lt;&gt;""),HYPERLINK(CONCATENATE(L2,B2),settings!$C$2),"")</calculatedColumnFormula>
+    <tableColumn id="5" name="date de création" dataDxfId="1">
+      <calculatedColumnFormula>VLOOKUP(B2,listing!$A$2:$E$700, 3, FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="date de modification" dataDxfId="2">
+      <calculatedColumnFormula>VLOOKUP(B2,listing!$A$2:$E$700, 4, FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" name="date d'accès" dataDxfId="3">
+      <calculatedColumnFormula>VLOOKUP(B2,listing!$A$2:$E$700, 5, FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="auteur" dataDxfId="10"/>
+    <tableColumn id="8" name="catégories" dataDxfId="9"/>
+    <tableColumn id="9" name="thèmes" dataDxfId="8"/>
+    <tableColumn id="10" name="statut" dataDxfId="7"/>
+    <tableColumn id="11" name="taille" dataDxfId="0">
+      <calculatedColumnFormula>VLOOKUP(B2,listing!$A$2:$E$700,2, FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" name="emplacement" dataDxfId="6"/>
+    <tableColumn id="13" name="afficher" dataDxfId="5" dataCellStyle="Lien hypertexte">
+      <calculatedColumnFormula>IF(AND(B2&lt;&gt;"",M2&lt;&gt;""),HYPERLINK(CONCATENATE(M2,B2),settings!$C$2),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -766,192 +1417,224 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil3"/>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="49" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="49" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="str">
+    <row r="2" spans="1:14" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="str">
         <f>IF(NOT(ISBLANK(B2)),CONCATENATE(settings!$A$2,settings!B2),"")</f>
         <v>DOC_1001</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="7">
-        <v>42741</v>
-      </c>
-      <c r="F2" s="7">
-        <v>42741</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="E2" s="13">
+        <f>VLOOKUP(B2,listing!$A$2:$E$700, 3, FALSE)</f>
+        <v>42741.917974537035</v>
+      </c>
+      <c r="F2" s="13">
+        <f>VLOOKUP(B2,listing!$A$2:$E$700, 4, FALSE)</f>
+        <v>42741.917974537035</v>
+      </c>
+      <c r="G2" s="13">
+        <f>VLOOKUP(B2,listing!$A$2:$E$700, 5, FALSE)</f>
+        <v>42741.917974537035</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="8">
         <v>1</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="8">
         <v>2</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="4">
-        <v>10</v>
-      </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="10">
+        <f>VLOOKUP(B2,listing!$A$2:$E$700,2, FALSE)</f>
+        <v>8339</v>
+      </c>
+      <c r="M2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="6" t="str">
-        <f>IF(AND(B2&lt;&gt;"",L2&lt;&gt;""),HYPERLINK(CONCATENATE(L2,B2),settings!$C$2),"")</f>
+      <c r="N2" s="11" t="str">
+        <f>IF(AND(B2&lt;&gt;"",M2&lt;&gt;""),HYPERLINK(CONCATENATE(M2,B2),settings!$C$2),"")</f>
         <v>Ouvrir le document</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="str">
+    <row r="3" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="str">
         <f>IF(NOT(ISBLANK(B3)),CONCATENATE(settings!$A$2,settings!B3),"")</f>
         <v>DOC_1002</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="5" t="str">
-        <f>IF(AND(B3&lt;&gt;"",L3&lt;&gt;""),HYPERLINK(CONCATENATE(L3,B3),settings!$C$2),"")</f>
+      <c r="B3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="13">
+        <f>VLOOKUP(B3,listing!$A$2:$E$700, 3, FALSE)</f>
+        <v>42741.943067129629</v>
+      </c>
+      <c r="F3" s="13">
+        <f>VLOOKUP(B3,listing!$A$2:$E$700, 4, FALSE)</f>
+        <v>42712.438969907409</v>
+      </c>
+      <c r="G3" s="13">
+        <f>VLOOKUP(B3,listing!$A$2:$E$700, 5, FALSE)</f>
+        <v>42741.943067129629</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="10">
+        <f>VLOOKUP(B3,listing!$A$2:$E$700,2, FALSE)</f>
+        <v>2287452</v>
+      </c>
+      <c r="M3" s="10"/>
+      <c r="N3" s="12" t="str">
+        <f>IF(AND(B3&lt;&gt;"",M3&lt;&gt;""),HYPERLINK(CONCATENATE(M3,B3),settings!$C$2),"")</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="str">
+    <row r="4" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="str">
         <f>IF(NOT(ISBLANK(B4)),CONCATENATE(settings!$A$2,settings!B4),"")</f>
         <v>DOC_1003</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="5" t="str">
-        <f>IF(AND(B4&lt;&gt;"",L4&lt;&gt;""),HYPERLINK(CONCATENATE(L4,B4),settings!$C$2),"")</f>
+      <c r="B4" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="13">
+        <f>VLOOKUP(B4,listing!$A$2:$E$700, 3, FALSE)</f>
+        <v>42741.943067129629</v>
+      </c>
+      <c r="F4" s="13">
+        <f>VLOOKUP(B4,listing!$A$2:$E$700, 4, FALSE)</f>
+        <v>42715.43822916667</v>
+      </c>
+      <c r="G4" s="13">
+        <f>VLOOKUP(B4,listing!$A$2:$E$700, 5, FALSE)</f>
+        <v>42741.943067129629</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="10">
+        <f>VLOOKUP(B4,listing!$A$2:$E$700,2, FALSE)</f>
+        <v>579144</v>
+      </c>
+      <c r="M4" s="10"/>
+      <c r="N4" s="12" t="str">
+        <f>IF(AND(B4&lt;&gt;"",M4&lt;&gt;""),HYPERLINK(CONCATENATE(M4,B4),settings!$C$2),"")</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="str">
-        <f>IF(NOT(ISBLANK(B5)),CONCATENATE(settings!$A$2,settings!B5),"")</f>
-        <v>DOC_1004</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="5" t="str">
-        <f>IF(AND(B5&lt;&gt;"",L5&lt;&gt;""),HYPERLINK(CONCATENATE(L5,B5),settings!$C$2),"")</f>
-        <v/>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="M2:M5">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Ouvrir le document">
-      <formula>NOT(ISERROR(SEARCH("Ouvrir le document",M2)))</formula>
+  <conditionalFormatting sqref="N2:N4">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Ouvrir le document">
+      <formula>NOT(ISERROR(SEARCH("Ouvrir le document",N2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5">
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4">
       <formula1>type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K4">
       <formula1>statut</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H4">
       <formula1>auteur</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4">
       <formula1>themes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I4">
       <formula1>categories</formula1>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F5">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F4 G3:G4">
       <formula1>42736</formula1>
       <formula2>43100</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B500">
+      <formula1>listingvba</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -962,28 +1645,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Feuil4"/>
-  <dimension ref="A3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:M500"/>
@@ -3683,4 +4344,222 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil4"/>
+  <dimension ref="A2:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2">
+        <v>2287452</v>
+      </c>
+      <c r="C2" s="4">
+        <v>42741.943067129629</v>
+      </c>
+      <c r="D2" s="4">
+        <v>42712.438969907409</v>
+      </c>
+      <c r="E2" s="4">
+        <v>42741.943067129629</v>
+      </c>
+      <c r="G2">
+        <f>COUNTA(A2:A65000)</f>
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3">
+        <v>579144</v>
+      </c>
+      <c r="C3" s="4">
+        <v>42741.943067129629</v>
+      </c>
+      <c r="D3" s="4">
+        <v>42715.43822916667</v>
+      </c>
+      <c r="E3" s="4">
+        <v>42741.943067129629</v>
+      </c>
+      <c r="F3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4">
+        <v>735598</v>
+      </c>
+      <c r="C4" s="4">
+        <v>42741.943067129629</v>
+      </c>
+      <c r="D4" s="4">
+        <v>42732.464641203704</v>
+      </c>
+      <c r="E4" s="4">
+        <v>42741.943067129629</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5">
+        <v>8339</v>
+      </c>
+      <c r="C5" s="4">
+        <v>42741.917974537035</v>
+      </c>
+      <c r="D5" s="4">
+        <v>42741.917974537035</v>
+      </c>
+      <c r="E5" s="4">
+        <v>42741.917974537035</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <v>566869</v>
+      </c>
+      <c r="C6" s="4">
+        <v>42741.943067129629</v>
+      </c>
+      <c r="D6" s="4">
+        <v>42715.892974537041</v>
+      </c>
+      <c r="E6" s="4">
+        <v>42741.943067129629</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7">
+        <v>5958548</v>
+      </c>
+      <c r="C7" s="4">
+        <v>42741.935104166667</v>
+      </c>
+      <c r="D7" s="4">
+        <v>42740.900393518517</v>
+      </c>
+      <c r="E7" s="4">
+        <v>42741.935104166667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8">
+        <v>191692</v>
+      </c>
+      <c r="C8" s="4">
+        <v>42741.935104166667</v>
+      </c>
+      <c r="D8" s="4">
+        <v>42740.881712962961</v>
+      </c>
+      <c r="E8" s="4">
+        <v>42741.935104166667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9">
+        <v>49137</v>
+      </c>
+      <c r="C9" s="4">
+        <v>42741.917974537035</v>
+      </c>
+      <c r="D9" s="4">
+        <v>42741.917974537035</v>
+      </c>
+      <c r="E9" s="4">
+        <v>42741.917974537035</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10">
+        <v>165</v>
+      </c>
+      <c r="C10" s="4">
+        <v>42741.952800925923</v>
+      </c>
+      <c r="D10" s="4">
+        <v>42741.952800925923</v>
+      </c>
+      <c r="E10" s="4">
+        <v>42741.952800925923</v>
+      </c>
+      <c r="F10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1026" r:id="rId4" name="Button 2">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!ListeFichiers">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>8</xdr:col>
+                    <xdr:colOff>752475</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+</worksheet>
 </file>
</xml_diff>